<commit_message>
Atualização automática de SANTA_VITORIA_DO_PALMAR.xlsx
</commit_message>
<xml_diff>
--- a/SANTA_VITORIA_DO_PALMAR.xlsx
+++ b/SANTA_VITORIA_DO_PALMAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E7670FF-FC4F-478E-BC89-82423036D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B63D8CED-080F-4FE1-835F-D65D5EA42ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1220,7 +1220,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B6F4BDD9-ED9B-4259-9EF4-D7787115E959}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{CE66E6DA-4CD6-4910-8FF4-B549ECBEB1A9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1250,10 +1250,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A2DD8B6-7828-40B2-80CB-F23FA564ABB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{645DC42F-FDBC-4A9B-815C-BBB281880E6B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1291,7 +1291,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380289F1-9FE0-4F64-B774-66DBD36BDE8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60006DC-E39C-41FD-B33C-561329746EA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1354,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA9C35E6-8B23-42DF-A7F9-54A26452E49D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8868816-76E5-4D3E-8EA7-92CA9060F85C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1373,7 +1373,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{344E03AD-4285-44AB-0E37-0D101CAC6881}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07C0E15D-B26F-38A3-9981-8AF51814790A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC0DB46-E00D-7A08-A9B7-7AEB9D888728}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4265129D-9AEA-06B1-88EB-821C5A097D1F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1441,7 +1441,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9F7F9E-D9FD-CCA5-9E39-E7380642F2D4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8510570-DEB9-5A57-229D-DFFED56F85D8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1472,7 +1472,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB1C75D6-D0CC-2C7A-2781-B6997CFD29D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BE06520-1FC9-BC8F-BB17-9FAA34CBA741}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1503,7 +1503,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B7D788D-0FF2-F484-BAF8-1F0E018D5C12}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3860A5E7-1BED-D749-634F-2B582DA1163D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1546,7 +1546,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D87FC64-0FB7-4272-8113-92A9835926A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632F8D9F-8331-40F8-9F7A-08375E7DBF5F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1584,7 +1584,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65047BF0-BC17-44C8-9245-605E4AD31C52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD09B9ED-347E-415E-A93D-5B0D07F8427C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1627,7 +1627,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99A653A0-7B65-4F3F-BECE-D8E9AF9B62D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E35EE784-9585-4AB4-A6AA-69628F01F77B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1940,7 +1940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DC77D1-D628-4A8B-B916-62139EAD42D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3792BA8-606F-43CE-9B8F-6B472EF2CF1E}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>